<commit_message>
app design changes to account for pipe variation
</commit_message>
<xml_diff>
--- a/Enid Purdy pipeline.xlsx
+++ b/Enid Purdy pipeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\CO2 TRANSPORT NETWORK MODEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E90D06-6D43-4F8E-849D-64FC5A8DEA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B19959-6649-4868-81C1-DB64FBFD697B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{7D3FBEBC-D24A-4E25-953F-F9EA23A735D7}"/>
   </bookViews>
@@ -454,7 +454,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>